<commit_message>
Updating respository for live commits
</commit_message>
<xml_diff>
--- a/BCRED/all_filings.xlsx
+++ b/BCRED/all_filings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanuthuppan/Downloads/RA Finance/BCRED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanuthuppan/Downloads/**RA Finance**/sec-scraper/BCRED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691AD5E5-6C74-8D42-A64C-9B83F2FA8B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D1264A-5AC3-5B46-B756-DA855D6F7C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="540" windowWidth="25600" windowHeight="16140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25600" windowHeight="16140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Form type</t>
   </si>
@@ -86,13 +86,25 @@
   </si>
   <si>
     <t>html_link</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349823000017/bcred-20230630.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349823000021/bcred-20230930.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349824000007/bcred-20231231.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349824000022/bcred-20240331.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -105,6 +117,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -126,16 +145,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -152,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -298,7 +321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -440,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -448,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -486,72 +509,72 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45056</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45016</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>45425</v>
+      </c>
+      <c r="D2" s="4">
+        <v>45382</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2">
-        <v>45002</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44926</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="4">
+        <v>45366</v>
+      </c>
+      <c r="D3" s="4">
+        <v>45291</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>44879</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44834</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="4">
+        <v>45243</v>
+      </c>
+      <c r="D4" s="4">
+        <v>45199</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
-        <v>44785</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44742</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
+      <c r="C5" s="4">
+        <v>45149</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45107</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -562,13 +585,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>44694</v>
+        <v>45056</v>
       </c>
       <c r="D6" s="2">
-        <v>44651</v>
+        <v>45016</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -579,13 +602,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>44629</v>
+        <v>45002</v>
       </c>
       <c r="D7" s="2">
-        <v>44561</v>
+        <v>44926</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -596,13 +619,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="2">
-        <v>44515</v>
+        <v>44879</v>
       </c>
       <c r="D8" s="2">
-        <v>44469</v>
+        <v>44834</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -613,13 +636,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>44424</v>
+        <v>44785</v>
       </c>
       <c r="D9" s="2">
-        <v>44377</v>
+        <v>44742</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -630,13 +653,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="2">
-        <v>44326</v>
+        <v>44694</v>
       </c>
       <c r="D10" s="2">
-        <v>44286</v>
+        <v>44651</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -647,13 +670,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="2">
-        <v>44260</v>
+        <v>44629</v>
       </c>
       <c r="D11" s="2">
-        <v>44196</v>
+        <v>44561</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -664,16 +687,90 @@
         <v>3</v>
       </c>
       <c r="C12" s="2">
+        <v>44515</v>
+      </c>
+      <c r="D12" s="2">
+        <v>44469</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2">
+        <v>44424</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44377</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="2">
+        <v>44326</v>
+      </c>
+      <c r="D14" s="2">
+        <v>44286</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
+        <v>44260</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44196</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
         <v>44151</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D16" s="2">
         <v>44104</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E16" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1A72F5D8-68E2-9A44-A49E-D7F5A655F0C5}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{2E564DC1-0A30-7342-9D8C-851E5416395A}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{4C97A781-1A11-8C47-81D0-75B7BA5C1DE9}"/>
+    <hyperlink ref="E12" r:id="rId4" xr:uid="{78C81769-84C6-DD45-A8ED-FDC817B4B58C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BCRED code finalized and MVC initial extraction done
</commit_message>
<xml_diff>
--- a/BCRED/all_filings.xlsx
+++ b/BCRED/all_filings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanuthuppan/Downloads/**RA Finance**/sec-scraper/BCRED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanuthuppan/Downloads/RA/BDC Cleaning/sec-scraper/BCRED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D1264A-5AC3-5B46-B756-DA855D6F7C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A4FAE0-2BD9-E841-A46C-5EEDCEC14A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25600" windowHeight="16140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>Form type</t>
   </si>
@@ -34,51 +34,12 @@
     <t>Quarterly report [Sections 13 or 15(d)]</t>
   </si>
   <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349823000012/0001803498-23-000012-index.htm</t>
-  </si>
-  <si>
     <t>10-K</t>
   </si>
   <si>
     <t>Annual report [Section 13 and 15(d), not S-K Item 405]</t>
   </si>
   <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349823000008/0001803498-23-000008-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000021/0001803498-22-000021-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000017/0001803498-22-000017-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000013/0001803498-22-000013-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000009/0001803498-22-000009-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349821000012/0001803498-21-000012-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349821000009/0001803498-21-000009-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349821000003/0001803498-21-000003-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000119312521069991/0001193125-21-069991-index.htm</t>
-  </si>
-  <si>
-    <t>https://www.sec.gov/Archives/edgar/data/1803498/000119312520294937/0001193125-20-294937-index.htm</t>
-  </si>
-  <si>
-    <t>total_investments_cost</t>
-  </si>
-  <si>
-    <t>total_investments_fv</t>
-  </si>
-  <si>
     <t>date_filed</t>
   </si>
   <si>
@@ -98,6 +59,42 @@
   </si>
   <si>
     <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349824000022/bcred-20240331.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349824000044/bcred-20240630.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349823000012/bcred-20230331.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349823000008/bcred-20221231.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000021/bcred-20220930.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000017/bcred-20220630.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000013/bcred-03312022x10q.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349822000009/bcred-20211231x10k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349821000012/bcred-09302021x10q.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349821000009/bcred-06302021x10q.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000180349821000003/bcred-03312021x10q.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000119312521069991/d145785d10k.htm</t>
+  </si>
+  <si>
+    <t>https://www.sec.gov/Archives/edgar/data/1803498/000119312520294937/d50632d10q.htm</t>
   </si>
 </sst>
 </file>
@@ -471,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -494,20 +491,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>18</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -517,47 +510,47 @@
         <v>3</v>
       </c>
       <c r="C2" s="4">
-        <v>45425</v>
+        <v>45517</v>
       </c>
       <c r="D2" s="4">
-        <v>45382</v>
+        <v>45473</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="C3" s="4">
-        <v>45366</v>
+        <v>45425</v>
       </c>
       <c r="D3" s="4">
-        <v>45291</v>
+        <v>45382</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4">
-        <v>45243</v>
+        <v>45366</v>
       </c>
       <c r="D4" s="4">
-        <v>45199</v>
+        <v>45291</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -568,64 +561,64 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
+        <v>45243</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45199</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
         <v>45149</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D6" s="4">
         <v>45107</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45056</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45016</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>45002</v>
+        <v>45056</v>
       </c>
       <c r="D7" s="2">
-        <v>44926</v>
+        <v>45016</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2">
-        <v>44879</v>
+        <v>45002</v>
       </c>
       <c r="D8" s="2">
-        <v>44834</v>
+        <v>44926</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -636,13 +629,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>44785</v>
+        <v>44879</v>
       </c>
       <c r="D9" s="2">
-        <v>44742</v>
+        <v>44834</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -653,47 +646,47 @@
         <v>3</v>
       </c>
       <c r="C10" s="2">
-        <v>44694</v>
+        <v>44785</v>
       </c>
       <c r="D10" s="2">
-        <v>44651</v>
+        <v>44742</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
-        <v>44629</v>
+        <v>44694</v>
       </c>
       <c r="D11" s="2">
-        <v>44561</v>
+        <v>44651</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
-        <v>44515</v>
+        <v>44629</v>
       </c>
       <c r="D12" s="2">
-        <v>44469</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
+        <v>44561</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -704,13 +697,13 @@
         <v>3</v>
       </c>
       <c r="C13" s="2">
-        <v>44424</v>
+        <v>44515</v>
       </c>
       <c r="D13" s="2">
-        <v>44377</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
+        <v>44469</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -721,55 +714,71 @@
         <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>44326</v>
+        <v>44424</v>
       </c>
       <c r="D14" s="2">
-        <v>44286</v>
+        <v>44377</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
-        <v>44260</v>
+        <v>44326</v>
       </c>
       <c r="D15" s="2">
-        <v>44196</v>
+        <v>44286</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2">
+        <v>44260</v>
+      </c>
+      <c r="D16" s="2">
+        <v>44196</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="2">
         <v>44151</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="2">
         <v>44104</v>
       </c>
-      <c r="E16" t="s">
-        <v>16</v>
+      <c r="E17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1A72F5D8-68E2-9A44-A49E-D7F5A655F0C5}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{2E564DC1-0A30-7342-9D8C-851E5416395A}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{4C97A781-1A11-8C47-81D0-75B7BA5C1DE9}"/>
-    <hyperlink ref="E12" r:id="rId4" xr:uid="{78C81769-84C6-DD45-A8ED-FDC817B4B58C}"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{1A72F5D8-68E2-9A44-A49E-D7F5A655F0C5}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{2E564DC1-0A30-7342-9D8C-851E5416395A}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{4C97A781-1A11-8C47-81D0-75B7BA5C1DE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>